<commit_message>
Realización de la pantalla excel dalta query solo
</commit_message>
<xml_diff>
--- a/APP/API/Excel/plantillasEXCEL/access.xlsx
+++ b/APP/API/Excel/plantillasEXCEL/access.xlsx
@@ -122,7 +122,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -131,7 +131,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -321,36 +329,39 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="1" width="28.09"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="1" width="8.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="8.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1025" style="2" width="8.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D3" s="4"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>